<commit_message>
modify block data type
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Block.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Block.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NF\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -99,10 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SpritePath</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -140,6 +139,10 @@
   </si>
   <si>
     <t>TreeRootList</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -194,8 +197,36 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -539,7 +570,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -600,7 +631,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -629,7 +660,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -661,7 +692,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -949,7 +980,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -981,7 +1012,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
@@ -1013,7 +1044,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1045,7 +1076,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -1077,7 +1108,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -1106,7 +1137,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -1135,7 +1166,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
@@ -1164,7 +1195,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
@@ -1193,7 +1224,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Change Excel Field View to Cache, And set default value to FALSE
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Block.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Block.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NF\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -22,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
   <si>
     <t>Id</t>
   </si>
@@ -39,7 +34,7 @@
     <t>Save</t>
   </si>
   <si>
-    <t>View</t>
+    <t>Cache</t>
   </si>
   <si>
     <t>Index</t>
@@ -60,69 +55,58 @@
     <t>Includes</t>
   </si>
   <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>Friend</t>
   </si>
   <si>
+    <t>SpriteList</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
+    <t>SpritePath</t>
+  </si>
+  <si>
     <t>LeftSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RightSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TopSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DownSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LeftTopSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LeftDownSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RightTopSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RightDownSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpritePath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpriteList</t>
   </si>
   <si>
     <t>LeftTopOutSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LeftDownOutSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RightTopOutSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RightDownOutSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GrassList</t>
@@ -135,44 +119,375 @@
   </si>
   <si>
     <t>TreasureList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TreeRootList</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -180,9 +495,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -194,47 +751,81 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFD7D7D7"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
+      <font/>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
+    <tableStyle name="MySqlDefault" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -284,71 +875,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -566,14 +1157,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F2" sqref="F2:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="8.25" customWidth="1"/>
@@ -588,7 +1180,7 @@
     <col min="12" max="12" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -626,12 +1218,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -643,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -652,18 +1244,18 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -675,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -684,18 +1276,18 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -707,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -716,18 +1308,18 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -739,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -748,18 +1340,18 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -771,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -780,19 +1372,19 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
@@ -803,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -812,18 +1404,18 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -835,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -844,18 +1436,18 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -867,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -876,18 +1468,18 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -899,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -908,18 +1500,18 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -931,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -940,18 +1532,18 @@
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -963,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -972,18 +1564,18 @@
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -995,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1004,18 +1596,18 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1027,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1036,18 +1628,18 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1059,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1068,18 +1660,18 @@
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1091,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1100,18 +1692,18 @@
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1123,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1132,15 +1724,15 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1152,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1161,15 +1753,15 @@
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1181,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1190,15 +1782,15 @@
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1210,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1219,15 +1811,15 @@
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1239,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1248,19 +1840,18 @@
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F21 F22:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>